<commit_message>
Lecture Excel et Enregistrement JSON done
</commit_message>
<xml_diff>
--- a/PlanningSandbox.xlsx
+++ b/PlanningSandbox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a490776a08fd031/Documents/EPF S6/Swish/BotMail/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="8_{C93A66CF-DF5D-456B-BE79-AF8969817D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A81B4E79-EE81-4478-AB8B-5B91CB2BD98C}"/>
+  <xr:revisionPtr revIDLastSave="170" documentId="8_{C93A66CF-DF5D-456B-BE79-AF8969817D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{594E8FD5-DF10-4C0A-A48D-284A5F931F13}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{16EB6ED4-2E25-4642-8164-370FEBA71D91}"/>
   </bookViews>
@@ -274,10 +274,6 @@
     <t>Périodicité en mois</t>
   </si>
   <si>
-    <t>Date de mise
- en service</t>
-  </si>
-  <si>
     <t>Bornes Simples</t>
   </si>
   <si>
@@ -410,6 +406,9 @@
   </si>
   <si>
     <t>Albert Albert2</t>
+  </si>
+  <si>
+    <t>Date de mise en service</t>
   </si>
 </sst>
 </file>
@@ -1617,7 +1616,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,7 +1630,8 @@
     <col min="7" max="7" width="28" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="40.140625" customWidth="1"/>
-    <col min="10" max="11" width="24.7109375" customWidth="1"/>
+    <col min="10" max="10" width="38.42578125" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" customWidth="1"/>
     <col min="12" max="12" width="28" customWidth="1"/>
     <col min="13" max="14" width="24.7109375" style="50" customWidth="1"/>
     <col min="15" max="15" width="21.28515625" style="52" customWidth="1"/>
@@ -1668,13 +1668,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="63" t="s">
         <v>72</v>
-      </c>
-      <c r="D3" s="64" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="63" t="s">
-        <v>73</v>
       </c>
       <c r="F3" s="65" t="s">
         <v>1</v>
@@ -1689,7 +1689,7 @@
         <v>63</v>
       </c>
       <c r="J3" s="65" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="K3" s="65" t="s">
         <v>2</v>
@@ -1731,10 +1731,10 @@
       </c>
       <c r="B4" s="34"/>
       <c r="C4" s="37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E4" s="37">
         <v>1</v>
@@ -1749,7 +1749,7 @@
         <v>4</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J4" s="2">
         <v>44557</v>
@@ -1791,10 +1791,10 @@
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" s="37">
         <v>2</v>
@@ -1809,7 +1809,7 @@
         <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J5" s="2">
         <v>44623</v>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="B6" s="34"/>
       <c r="C6" s="37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" s="37">
         <v>0</v>
@@ -1863,7 +1863,7 @@
         <v>6</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J6" s="2">
         <v>44743</v>
@@ -1899,10 +1899,10 @@
       </c>
       <c r="B7" s="34"/>
       <c r="C7" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="37" t="s">
         <v>78</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>79</v>
       </c>
       <c r="E7" s="37">
         <v>2</v>
@@ -1917,7 +1917,7 @@
         <v>7</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J7" s="2">
         <v>44668</v>
@@ -7176,6 +7176,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E948A9CE1FB2CE4C8AE9B70A9B9CE023" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb8a8860a1c4c91bbc706a6e17b12ecc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6b78c6ca-c81e-4330-9bb3-0f577d436514" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="33efc8288bb545af800450190bca8712" ns2:_="">
     <xsd:import namespace="6b78c6ca-c81e-4330-9bb3-0f577d436514"/>
@@ -7307,15 +7316,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F79E8CDE-DD09-4AC8-B0E1-24EB8300EF2F}">
   <ds:schemaRefs>
@@ -7333,6 +7333,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5F11FFB-EF31-444D-8074-B41CB27BA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D78C85D1-94BC-46D4-A9DE-737AD1712B15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7348,12 +7356,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5F11FFB-EF31-444D-8074-B41CB27BA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Envoi du mail près attente du serveur
</commit_message>
<xml_diff>
--- a/PlanningSandbox.xlsx
+++ b/PlanningSandbox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a490776a08fd031/Documents/EPF S6/Swish/BotMail/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="170" documentId="8_{C93A66CF-DF5D-456B-BE79-AF8969817D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{594E8FD5-DF10-4C0A-A48D-284A5F931F13}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="8_{C93A66CF-DF5D-456B-BE79-AF8969817D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9802E76F-CE1B-48D0-BF5D-115934130C53}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{16EB6ED4-2E25-4642-8164-370FEBA71D91}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
   <si>
     <t>N° Affaire</t>
   </si>
@@ -386,9 +386,6 @@
       </rPr>
       <t>)</t>
     </r>
-  </si>
-  <si>
-    <t>3 (ALFEN )</t>
   </si>
   <si>
     <t>Bornes Doubles</t>
@@ -1616,7 +1613,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1671,7 +1668,7 @@
         <v>71</v>
       </c>
       <c r="D3" s="64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="63" t="s">
         <v>72</v>
@@ -1689,7 +1686,7 @@
         <v>63</v>
       </c>
       <c r="J3" s="65" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K3" s="65" t="s">
         <v>2</v>
@@ -1749,7 +1746,7 @@
         <v>4</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J4" s="2">
         <v>44557</v>
@@ -1794,7 +1791,7 @@
         <v>74</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" s="37">
         <v>2</v>
@@ -1809,7 +1806,7 @@
         <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J5" s="2">
         <v>44623</v>
@@ -1863,7 +1860,7 @@
         <v>6</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J6" s="2">
         <v>44743</v>
@@ -1901,9 +1898,7 @@
       <c r="C7" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="37" t="s">
-        <v>78</v>
-      </c>
+      <c r="D7" s="37"/>
       <c r="E7" s="37">
         <v>2</v>
       </c>
@@ -1917,7 +1912,7 @@
         <v>7</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J7" s="2">
         <v>44668</v>
@@ -7176,15 +7171,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E948A9CE1FB2CE4C8AE9B70A9B9CE023" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb8a8860a1c4c91bbc706a6e17b12ecc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6b78c6ca-c81e-4330-9bb3-0f577d436514" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="33efc8288bb545af800450190bca8712" ns2:_="">
     <xsd:import namespace="6b78c6ca-c81e-4330-9bb3-0f577d436514"/>
@@ -7316,6 +7302,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F79E8CDE-DD09-4AC8-B0E1-24EB8300EF2F}">
   <ds:schemaRefs>
@@ -7333,14 +7328,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5F11FFB-EF31-444D-8074-B41CB27BA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D78C85D1-94BC-46D4-A9DE-737AD1712B15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7356,4 +7343,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5F11FFB-EF31-444D-8074-B41CB27BA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Version fonctionnelle du composant Editor
</commit_message>
<xml_diff>
--- a/PlanningSandbox.xlsx
+++ b/PlanningSandbox.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a490776a08fd031/Documents/EPF S6/Swish/BotMail/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1 Dossiers de Nicolas\Etudes EPF\Swish\Code\BotMail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="170" documentId="8_{C93A66CF-DF5D-456B-BE79-AF8969817D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{594E8FD5-DF10-4C0A-A48D-284A5F931F13}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3867D2E2-3BA4-4B95-AFAE-FAB68535E88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{16EB6ED4-2E25-4642-8164-370FEBA71D91}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{16EB6ED4-2E25-4642-8164-370FEBA71D91}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="2" r:id="rId1"/>
@@ -306,33 +306,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>3 (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ALFEN EVE MINI MURALE
-ALFEN EVE DOUBLE PRO LINE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-  </si>
-  <si>
     <t>2 (ALFEN )</t>
   </si>
   <si>
@@ -409,6 +382,32 @@
   </si>
   <si>
     <t>Date de mise en service</t>
+  </si>
+  <si>
+    <r>
+      <t>3 (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALFEN EVE MINI MURALE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1315,7 +1314,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1614,35 +1613,35 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A2:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="65" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="40.140625" customWidth="1"/>
-    <col min="10" max="10" width="38.42578125" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" customWidth="1"/>
+    <col min="9" max="9" width="40.109375" customWidth="1"/>
+    <col min="10" max="10" width="38.44140625" customWidth="1"/>
+    <col min="11" max="11" width="24.6640625" customWidth="1"/>
     <col min="12" max="12" width="28" customWidth="1"/>
-    <col min="13" max="14" width="24.7109375" style="50" customWidth="1"/>
-    <col min="15" max="15" width="21.28515625" style="52" customWidth="1"/>
-    <col min="16" max="17" width="21.28515625" style="54" customWidth="1"/>
-    <col min="18" max="18" width="20.42578125" style="56" customWidth="1"/>
-    <col min="19" max="20" width="20.42578125" style="58" customWidth="1"/>
-    <col min="21" max="21" width="20.85546875" style="60" customWidth="1"/>
-    <col min="22" max="22" width="2.42578125" style="18" customWidth="1"/>
+    <col min="13" max="14" width="24.6640625" style="50" customWidth="1"/>
+    <col min="15" max="15" width="21.33203125" style="52" customWidth="1"/>
+    <col min="16" max="17" width="21.33203125" style="54" customWidth="1"/>
+    <col min="18" max="18" width="20.44140625" style="56" customWidth="1"/>
+    <col min="19" max="20" width="20.44140625" style="58" customWidth="1"/>
+    <col min="21" max="21" width="20.88671875" style="60" customWidth="1"/>
+    <col min="22" max="22" width="2.44140625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="63"/>
       <c r="B2" s="62"/>
       <c r="C2" s="72" t="s">
@@ -1660,7 +1659,7 @@
       <c r="M2" s="66"/>
       <c r="N2" s="66"/>
     </row>
-    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="63" t="s">
         <v>69</v>
       </c>
@@ -1671,7 +1670,7 @@
         <v>71</v>
       </c>
       <c r="D3" s="64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="63" t="s">
         <v>72</v>
@@ -1689,7 +1688,7 @@
         <v>63</v>
       </c>
       <c r="J3" s="65" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K3" s="65" t="s">
         <v>2</v>
@@ -1725,7 +1724,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
         <v>51</v>
       </c>
@@ -1734,7 +1733,7 @@
         <v>73</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" s="37">
         <v>1</v>
@@ -1749,10 +1748,10 @@
         <v>4</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J4" s="2">
-        <v>44557</v>
+        <v>44404</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="1">
@@ -1760,7 +1759,7 @@
       </c>
       <c r="M4" s="51">
         <f t="shared" ref="M4:M7" si="0">DATE(YEAR(J4)+1,MONTH(J4),DAY(J4))</f>
-        <v>44922</v>
+        <v>44769</v>
       </c>
       <c r="N4" s="51" t="s">
         <v>59</v>
@@ -1770,7 +1769,7 @@
       </c>
       <c r="P4" s="55">
         <f t="shared" ref="P4:P7" si="1">DATE(YEAR(J4)+2,MONTH(J4),DAY(J4))</f>
-        <v>45287</v>
+        <v>45134</v>
       </c>
       <c r="Q4" s="55" t="s">
         <v>59</v>
@@ -1778,23 +1777,23 @@
       <c r="R4" s="57"/>
       <c r="S4" s="59">
         <f>DATE(YEAR(J4)+3,MONTH(J4),DAY(J4))</f>
-        <v>45653</v>
+        <v>45500</v>
       </c>
       <c r="T4" s="59" t="s">
         <v>59</v>
       </c>
       <c r="U4" s="61"/>
     </row>
-    <row r="5" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
         <v>52</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="37" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" s="37">
         <v>2</v>
@@ -1809,10 +1808,10 @@
         <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J5" s="2">
-        <v>44623</v>
+        <v>44350</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="1">
@@ -1820,7 +1819,7 @@
       </c>
       <c r="M5" s="51">
         <f t="shared" si="0"/>
-        <v>44988</v>
+        <v>44715</v>
       </c>
       <c r="N5" s="51"/>
       <c r="O5" s="53">
@@ -1828,24 +1827,24 @@
       </c>
       <c r="P5" s="55">
         <f t="shared" si="1"/>
-        <v>45354</v>
+        <v>45080</v>
       </c>
       <c r="Q5" s="55"/>
       <c r="R5" s="57"/>
       <c r="S5" s="59">
         <f t="shared" ref="S5:S7" si="2">DATE(YEAR(J5)+3,MONTH(J5),DAY(J5))</f>
-        <v>45719</v>
+        <v>45446</v>
       </c>
       <c r="T5" s="59"/>
       <c r="U5" s="61"/>
     </row>
-    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
         <v>53</v>
       </c>
       <c r="B6" s="34"/>
       <c r="C6" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6" s="37">
         <v>0</v>
@@ -1863,10 +1862,10 @@
         <v>6</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J6" s="2">
-        <v>44743</v>
+        <v>44378</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="1">
@@ -1874,7 +1873,7 @@
       </c>
       <c r="M6" s="51">
         <f t="shared" si="0"/>
-        <v>45108</v>
+        <v>44743</v>
       </c>
       <c r="N6" s="51" t="s">
         <v>59</v>
@@ -1882,27 +1881,27 @@
       <c r="O6" s="53"/>
       <c r="P6" s="55">
         <f t="shared" si="1"/>
-        <v>45474</v>
+        <v>45108</v>
       </c>
       <c r="Q6" s="55"/>
       <c r="R6" s="57"/>
       <c r="S6" s="59">
         <f t="shared" si="2"/>
-        <v>45839</v>
+        <v>45474</v>
       </c>
       <c r="T6" s="59"/>
       <c r="U6" s="61"/>
     </row>
-    <row r="7" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="34"/>
       <c r="C7" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="37" t="s">
         <v>77</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>78</v>
       </c>
       <c r="E7" s="37">
         <v>2</v>
@@ -1917,10 +1916,10 @@
         <v>7</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J7" s="2">
-        <v>44668</v>
+        <v>44425</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="1">
@@ -1928,7 +1927,7 @@
       </c>
       <c r="M7" s="51">
         <f t="shared" si="0"/>
-        <v>45033</v>
+        <v>44790</v>
       </c>
       <c r="N7" s="51" t="s">
         <v>59</v>
@@ -1938,7 +1937,7 @@
       </c>
       <c r="P7" s="55">
         <f t="shared" si="1"/>
-        <v>45399</v>
+        <v>45155</v>
       </c>
       <c r="Q7" s="55" t="s">
         <v>59</v>
@@ -1946,7 +1945,7 @@
       <c r="R7" s="57"/>
       <c r="S7" s="59">
         <f t="shared" si="2"/>
-        <v>45764</v>
+        <v>45521</v>
       </c>
       <c r="T7" s="59"/>
       <c r="U7" s="61"/>
@@ -1973,64 +1972,64 @@
       <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="9"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="9"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="34" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="8" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="44" max="46" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="46" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="8" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="56" max="58" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="58" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="7.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
@@ -2108,7 +2107,7 @@
       <c r="BK1" s="86"/>
       <c r="BL1" s="86"/>
     </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>11</v>
       </c>
@@ -2302,7 +2301,7 @@
         <v>46357</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="str">
         <f>VLOOKUP(Clients!A4,Clients!A3:U7,1,FALSE)</f>
         <v>ENTREPRISE 1</v>
@@ -2317,7 +2316,7 @@
       </c>
       <c r="D3" s="15">
         <f>VLOOKUP(Clients!G4,Clients!G3:W7,7,FALSE)</f>
-        <v>44922</v>
+        <v>44769</v>
       </c>
       <c r="E3" s="6">
         <f>IF(MONTH($D3)&amp;YEAR($D3)=MONTH(E$2)&amp;YEAR(E$2),3,IF(MONTH($C3)&amp;YEAR($C3)=MONTH(E$2)&amp;YEAR(E$2),2,IF(MONTH($B3)&amp;YEAR($B3)=MONTH(E$2)&amp;YEAR(E$2),1,0)))</f>
@@ -2345,7 +2344,7 @@
       </c>
       <c r="K3" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L3" s="6">
         <f t="shared" si="0"/>
@@ -2365,7 +2364,7 @@
       </c>
       <c r="P3" s="24">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="27">
         <f t="shared" si="0"/>
@@ -2560,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="str">
         <f>VLOOKUP(Clients!A5,Clients!A4:U7,1,FALSE)</f>
         <v>ENTREPRISE 2</v>
@@ -2577,7 +2576,7 @@
       </c>
       <c r="D4" s="15">
         <f>VLOOKUP(Clients!G5,Clients!G4:W7,7,FALSE)</f>
-        <v>44988</v>
+        <v>44715</v>
       </c>
       <c r="E4" s="6" t="e">
         <f t="shared" ref="E4:E18" si="4">IF(MONTH($D4)&amp;YEAR($D4)=MONTH(E$2)&amp;YEAR(E$2),3,IF(MONTH($C4)&amp;YEAR($C4)=MONTH(E$2)&amp;YEAR(E$2),2,IF(MONTH($B4)&amp;YEAR($B4)=MONTH(E$2)&amp;YEAR(E$2),1,0)))</f>
@@ -2599,46 +2598,46 @@
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J4" s="6" t="e">
+      <c r="J4" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K4" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K4" s="6" t="e">
+      <c r="L4" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L4" s="6" t="e">
+      <c r="M4" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M4" s="6" t="e">
+      <c r="N4" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N4" s="6" t="e">
+      <c r="O4" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="O4" s="6" t="e">
+      <c r="P4" s="24" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="P4" s="24" t="e">
+      <c r="Q4" s="27" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q4" s="27" t="e">
+      <c r="R4" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="R4" s="6" t="e">
+      <c r="S4" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="S4" s="6">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
       <c r="T4" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
@@ -2820,7 +2819,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="str">
         <f>VLOOKUP(Clients!A6,Clients!A5:U7,1,FALSE)</f>
         <v>ENTREPRISE 3</v>
@@ -2835,7 +2834,7 @@
       </c>
       <c r="D5" s="15">
         <f>VLOOKUP(Clients!G6,Clients!G5:W7,7,FALSE)</f>
-        <v>45108</v>
+        <v>44743</v>
       </c>
       <c r="E5" s="6">
         <f t="shared" si="4"/>
@@ -2863,7 +2862,7 @@
       </c>
       <c r="K5" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" si="0"/>
@@ -2911,7 +2910,7 @@
       </c>
       <c r="W5" s="6">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X5" s="6">
         <f t="shared" si="1"/>
@@ -3078,7 +3077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="str">
         <f>VLOOKUP(Clients!A7,Clients!A6:U7,1,FALSE)</f>
         <v>ENTREPRISE 4</v>
@@ -3093,7 +3092,7 @@
       </c>
       <c r="D6" s="15">
         <f>VLOOKUP(Clients!G7,Clients!G6:W7,7,FALSE)</f>
-        <v>45033</v>
+        <v>44790</v>
       </c>
       <c r="E6" s="6">
         <f t="shared" si="4"/>
@@ -3125,7 +3124,7 @@
       </c>
       <c r="L6" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M6" s="6">
         <f t="shared" si="0"/>
@@ -3157,7 +3156,7 @@
       </c>
       <c r="T6" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U6" s="6">
         <f t="shared" si="0"/>
@@ -3336,7 +3335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!A7:U7,1,FALSE)</f>
         <v>#REF!</v>
@@ -3594,7 +3593,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -3852,7 +3851,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -4110,7 +4109,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -4368,7 +4367,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -4626,7 +4625,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -4884,7 +4883,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -5142,7 +5141,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -5400,7 +5399,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -5658,7 +5657,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -5916,7 +5915,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -6174,7 +6173,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -6432,7 +6431,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -6450,7 +6449,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -6468,7 +6467,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -6486,7 +6485,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -6504,7 +6503,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -6522,7 +6521,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -6540,7 +6539,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!#REF!,1,FALSE)</f>
         <v>#REF!</v>
@@ -6558,119 +6557,119 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
     </row>
   </sheetData>
@@ -6743,12 +6742,12 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="38">
         <v>1</v>
       </c>
@@ -6756,7 +6755,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="38">
         <v>2</v>
       </c>
@@ -6764,7 +6763,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="38">
         <v>3</v>
       </c>
@@ -6785,7 +6784,7 @@
       <c r="V4" s="41"/>
       <c r="W4" s="42"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="38">
         <v>4</v>
       </c>
@@ -6804,7 +6803,7 @@
       <c r="V5" s="44"/>
       <c r="W5" s="45"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="38">
         <v>5</v>
       </c>
@@ -6829,7 +6828,7 @@
       <c r="V6" s="44"/>
       <c r="W6" s="45"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="38">
         <v>6</v>
       </c>
@@ -6848,7 +6847,7 @@
       <c r="V7" s="44"/>
       <c r="W7" s="45"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="38">
         <v>7</v>
       </c>
@@ -6866,7 +6865,7 @@
       <c r="V8" s="44"/>
       <c r="W8" s="45"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="38">
         <v>8</v>
       </c>
@@ -6882,7 +6881,7 @@
       <c r="V9" s="44"/>
       <c r="W9" s="45"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="38">
         <v>9</v>
       </c>
@@ -6900,7 +6899,7 @@
       <c r="V10" s="44"/>
       <c r="W10" s="45"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="38">
         <v>10</v>
       </c>
@@ -6918,7 +6917,7 @@
       <c r="V11" s="44"/>
       <c r="W11" s="45"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="M12" s="43"/>
       <c r="N12" s="44"/>
       <c r="O12" s="44"/>
@@ -6931,7 +6930,7 @@
       <c r="V12" s="44"/>
       <c r="W12" s="45"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="M13" s="46" t="s">
         <v>27</v>
       </c>
@@ -6948,7 +6947,7 @@
       <c r="V13" s="44"/>
       <c r="W13" s="45"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="M14" s="46" t="s">
         <v>28</v>
       </c>
@@ -6965,7 +6964,7 @@
       <c r="V14" s="44"/>
       <c r="W14" s="45"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="M15" s="46" t="s">
         <v>30</v>
       </c>
@@ -6982,7 +6981,7 @@
       <c r="V15" s="44"/>
       <c r="W15" s="45"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="M16" s="43"/>
       <c r="N16" s="44"/>
       <c r="O16" s="44"/>
@@ -6995,7 +6994,7 @@
       <c r="V16" s="44"/>
       <c r="W16" s="45"/>
     </row>
-    <row r="17" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="13:23" x14ac:dyDescent="0.3">
       <c r="M17" s="43"/>
       <c r="N17" s="44"/>
       <c r="O17" s="44"/>
@@ -7008,7 +7007,7 @@
       <c r="V17" s="44"/>
       <c r="W17" s="45"/>
     </row>
-    <row r="18" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="13:23" x14ac:dyDescent="0.3">
       <c r="M18" s="43" t="s">
         <v>32</v>
       </c>
@@ -7023,7 +7022,7 @@
       <c r="V18" s="44"/>
       <c r="W18" s="45"/>
     </row>
-    <row r="19" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="13:23" x14ac:dyDescent="0.3">
       <c r="M19" s="43"/>
       <c r="N19" s="44"/>
       <c r="O19" s="44"/>
@@ -7036,7 +7035,7 @@
       <c r="V19" s="44"/>
       <c r="W19" s="45"/>
     </row>
-    <row r="20" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="13:23" x14ac:dyDescent="0.3">
       <c r="M20" s="43" t="s">
         <v>33</v>
       </c>
@@ -7051,7 +7050,7 @@
       <c r="V20" s="44"/>
       <c r="W20" s="45"/>
     </row>
-    <row r="21" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="13:23" x14ac:dyDescent="0.3">
       <c r="M21" s="47"/>
       <c r="N21" s="48"/>
       <c r="O21" s="48"/>
@@ -7079,13 +7078,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
@@ -7094,7 +7093,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -7102,7 +7101,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -7110,7 +7109,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -7118,7 +7117,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -7126,32 +7125,32 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Gestion des oublis d'espace dans les bornes
</commit_message>
<xml_diff>
--- a/PlanningSandbox.xlsx
+++ b/PlanningSandbox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a490776a08fd031/Documents/EPF S6/Swish/BotMail/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{3867D2E2-3BA4-4B95-AFAE-FAB68535E88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF01FEFC-0E54-400F-9E1A-63B56A6A3ED6}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{3867D2E2-3BA4-4B95-AFAE-FAB68535E88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{687653F8-9A05-42E5-ABE5-8DD7B754A300}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{16EB6ED4-2E25-4642-8164-370FEBA71D91}"/>
   </bookViews>
@@ -272,32 +272,6 @@
     <t>Armoires</t>
   </si>
   <si>
-    <r>
-      <t>4 (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ALFEN EVE SINGLE PRO LINE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>2 (ALFEN )</t>
   </si>
   <si>
@@ -556,6 +530,32 @@
   <si>
     <t>2 rue Albert Albert
 78700, Colombes</t>
+  </si>
+  <si>
+    <r>
+      <t>4                (A</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LFEN EVE SINGLE PRO LINE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1294,6 +1294,24 @@
   <dxfs count="13">
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="2"/>
       </font>
       <fill>
@@ -1412,24 +1430,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1452,7 +1452,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9164956E-0D69-4620-BD79-986171F62F35}" name="Tableau1" displayName="Tableau1" ref="A1:A11" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9164956E-0D69-4620-BD79-986171F62F35}" name="Tableau1" displayName="Tableau1" ref="A1:A11" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:A11" xr:uid="{9164956E-0D69-4620-BD79-986171F62F35}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{67E9F617-4712-4E72-89F0-4AE05707B1FB}" name="Statut"/>
@@ -1762,8 +1762,8 @@
   <dimension ref="A2:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1818,7 +1818,7 @@
         <v>69</v>
       </c>
       <c r="D3" s="64" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3" s="63" t="s">
         <v>70</v>
@@ -1836,7 +1836,7 @@
         <v>61</v>
       </c>
       <c r="J3" s="65" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K3" s="65" t="s">
         <v>2</v>
@@ -1878,10 +1878,10 @@
       </c>
       <c r="B4" s="34"/>
       <c r="C4" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="37" t="s">
         <v>71</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>72</v>
       </c>
       <c r="E4" s="37">
         <v>1</v>
@@ -1890,13 +1890,13 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J4" s="2">
         <v>44404</v>
@@ -1938,10 +1938,10 @@
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" s="37">
         <v>2</v>
@@ -1950,13 +1950,13 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J5" s="2">
         <v>44350</v>
@@ -1992,7 +1992,7 @@
       </c>
       <c r="B6" s="34"/>
       <c r="C6" s="37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="37">
         <v>0</v>
@@ -2010,7 +2010,7 @@
         <v>6</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J6" s="2">
         <v>44378</v>
@@ -2046,10 +2046,10 @@
       </c>
       <c r="B7" s="34"/>
       <c r="C7" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="37" t="s">
         <v>74</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>75</v>
       </c>
       <c r="E7" s="37">
         <v>2</v>
@@ -2061,10 +2061,10 @@
         <v>56</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J7" s="2">
         <v>44425</v>
@@ -2100,11 +2100,11 @@
     </row>
     <row r="8" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="34"/>
       <c r="C8" s="37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="37">
         <v>0</v>
@@ -2116,13 +2116,13 @@
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J8" s="2">
         <v>44472</v>
@@ -2154,14 +2154,14 @@
     </row>
     <row r="9" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" s="34"/>
       <c r="C9" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="37" t="s">
         <v>88</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>89</v>
       </c>
       <c r="E9" s="37">
         <v>6</v>
@@ -2170,13 +2170,13 @@
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J9" s="2">
         <v>44519</v>
@@ -2212,11 +2212,11 @@
     </row>
     <row r="10" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="34"/>
       <c r="C10" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10" s="37">
         <v>0</v>
@@ -2228,13 +2228,13 @@
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J10" s="2">
         <v>44566</v>
@@ -2266,14 +2266,14 @@
     </row>
     <row r="11" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="34"/>
       <c r="C11" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="37" t="s">
         <v>96</v>
-      </c>
-      <c r="D11" s="37" t="s">
-        <v>97</v>
       </c>
       <c r="E11" s="37">
         <v>10</v>
@@ -2282,13 +2282,13 @@
         <v>3</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J11" s="2">
         <v>44613</v>
@@ -7059,44 +7059,44 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:BL16">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17:BL17">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:BL18">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7547,15 +7547,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E948A9CE1FB2CE4C8AE9B70A9B9CE023" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb8a8860a1c4c91bbc706a6e17b12ecc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6b78c6ca-c81e-4330-9bb3-0f577d436514" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="33efc8288bb545af800450190bca8712" ns2:_="">
     <xsd:import namespace="6b78c6ca-c81e-4330-9bb3-0f577d436514"/>
@@ -7687,6 +7678,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F79E8CDE-DD09-4AC8-B0E1-24EB8300EF2F}">
   <ds:schemaRefs>
@@ -7704,14 +7704,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5F11FFB-EF31-444D-8074-B41CB27BA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D78C85D1-94BC-46D4-A9DE-737AD1712B15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7727,4 +7719,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5F11FFB-EF31-444D-8074-B41CB27BA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>